<commit_message>
Added possibility of running models with different time resolutions
</commit_message>
<xml_diff>
--- a/output/line_data.xlsx
+++ b/output/line_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vegardvk\vscodeProjects\bernstein\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA9943B-BEF2-46B3-BBAA-E0CA4CB27BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EB57B6-4A0E-4B85-A64D-862678602984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="38040" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="19185" windowHeight="10200" xr2:uid="{DC188162-EFF5-47E3-B49E-82E8905BA224}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>